<commit_message>
add working heatmap code and the data matrix.
</commit_message>
<xml_diff>
--- a/Calibration Plots.xlsx
+++ b/Calibration Plots.xlsx
@@ -5,20 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psadhwani\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olincollege-my.sharepoint.com/personal/jzeng_olin_edu/Documents/2021 Fall/POE/DIY-3D-Scanner/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{EF4CB82D-8EE5-4CE4-A3B7-7918C0317ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7BA09604-5152-43EC-8FB5-A6829332C1EB}"/>
+    <workbookView minimized="1" xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7875" xr2:uid="{7BA09604-5152-43EC-8FB5-A6829332C1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$14</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -151,9 +147,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Calibration</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -2663,7 +2656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046A7345-9349-4A52-A704-D65B70B6C199}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="97" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add random plot points
</commit_message>
<xml_diff>
--- a/Calibration Plots.xlsx
+++ b/Calibration Plots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olincollege-my.sharepoint.com/personal/jzeng_olin_edu/Documents/2021 Fall/POE/DIY-3D-Scanner/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psadhwani\Downloads\DIY-3D-Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF4CB82D-8EE5-4CE4-A3B7-7918C0317ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F40AC-78F2-4240-A31B-DC2AA515EE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1470" yWindow="1470" windowWidth="15375" windowHeight="7875" xr2:uid="{7BA09604-5152-43EC-8FB5-A6829332C1EB}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{7BA09604-5152-43EC-8FB5-A6829332C1EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -147,6 +147,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Output</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -221,10 +232,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -263,16 +274,25 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>567</c:v>
                 </c:pt>
@@ -311,6 +331,15 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>542</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,10 +783,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>567</c:v>
                 </c:pt>
@@ -796,16 +825,25 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>542</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>240</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
@@ -844,6 +882,15 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2347,8 +2394,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A34FDE9D-6D02-4134-BFA8-5A8CADEF7388}" name="Table1" displayName="Table1" ref="A1:B14" totalsRowShown="0">
-  <autoFilter ref="A1:B14" xr:uid="{A34FDE9D-6D02-4134-BFA8-5A8CADEF7388}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A34FDE9D-6D02-4134-BFA8-5A8CADEF7388}" name="Table1" displayName="Table1" ref="A1:B17" totalsRowShown="0">
+  <autoFilter ref="A1:B17" xr:uid="{A34FDE9D-6D02-4134-BFA8-5A8CADEF7388}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{58C290BD-6DBC-4228-9EE5-2A4C5B674609}" name="Distance"/>
     <tableColumn id="2" xr3:uid="{001E8114-091B-4403-9CE6-73669ADCA6BC}" name="Output"/>
@@ -2654,10 +2701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046A7345-9349-4A52-A704-D65B70B6C199}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2778,6 +2825,30 @@
         <v>175</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>240</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>